<commit_message>
added january excel data
</commit_message>
<xml_diff>
--- a/media/excels/1-6consumer_price_index1.xlsx
+++ b/media/excels/1-6consumer_price_index1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\work\macrobulletin_project\media\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55843D52-ED74-4869-9732-B9242CB4F88E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC12CC73-8842-465D-95F6-4C191773A351}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
   <si>
     <t>Показатели</t>
   </si>
@@ -73,6 +73,9 @@
     <t>ноя</t>
   </si>
   <si>
+    <t>дек</t>
+  </si>
+  <si>
     <t>Потребительские цены</t>
   </si>
   <si>
@@ -115,6 +118,9 @@
     <t>110.3</t>
   </si>
   <si>
+    <t>109.8</t>
+  </si>
+  <si>
     <t>Продовольственные товары</t>
   </si>
   <si>
@@ -154,12 +160,12 @@
     <t>109.2</t>
   </si>
   <si>
+    <t>108.5</t>
+  </si>
+  <si>
     <t>Непродовольственные товары</t>
   </si>
   <si>
-    <t>108.5</t>
-  </si>
-  <si>
     <t>119.4</t>
   </si>
   <si>
@@ -184,6 +190,9 @@
     <t>111.1</t>
   </si>
   <si>
+    <t>109.1</t>
+  </si>
+  <si>
     <t>Платные услуги</t>
   </si>
   <si>
@@ -260,6 +269,9 @@
   </si>
   <si>
     <t>104.8</t>
+  </si>
+  <si>
+    <t>102</t>
   </si>
 </sst>
 </file>
@@ -639,15 +651,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:N1"/>
+      <selection activeCell="D1" sqref="D1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -670,8 +682,9 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -714,234 +727,252 @@
       <c r="N2" t="s">
         <v>16</v>
       </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" t="s">
-        <v>30</v>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
+    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s">
         <v>41</v>
       </c>
-      <c r="M4" t="s">
+      <c r="I6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" t="s">
         <v>42</v>
       </c>
-      <c r="N4" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="M7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="N7" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="O7" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="D1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:N7 A1:D1" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:O7 A1:D1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>